<commit_message>
modified app to Class
</commit_message>
<xml_diff>
--- a/excel.xlsx
+++ b/excel.xlsx
@@ -1,18 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\INTERCEPT\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11544" windowHeight="5556"/>
   </bookViews>
   <sheets>
-    <sheet name="POSITIONS" sheetId="1" r:id="rId3"/>
+    <sheet name="POSITIONS" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="41">
   <si>
     <t/>
   </si>
@@ -140,73 +147,36 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts/>
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color indexed="8"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
-      <color rgb="000000"/>
-      <sz val="11"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <color rgb="000000"/>
-      <sz val="11"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <b/>
-      <color rgb="FFFFFF"/>
-      <sz val="11"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <b/>
-      <color rgb="000000"/>
-      <sz val="11"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="darkGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00FFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00FFDDDD"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00041957"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00FFFFE0"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="0000FFFF"/>
+        <fgColor rgb="FF041957"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -214,81 +184,337 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="00FF0000"/>
-      </left>
-      <right style="thin">
-        <color rgb="00FF0000"/>
-      </right>
-      <top style="thin">
-        <color rgb="00FF0000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="00FF0000"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="true" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4472C4"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView tabSelected="true" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:XFD15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -323,7 +549,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -358,7 +584,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -393,7 +619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -428,7 +654,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>29</v>
       </c>
@@ -463,7 +689,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>33</v>
       </c>
@@ -498,7 +724,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>36</v>
       </c>
@@ -530,6 +756,251 @@
         <v>0</v>
       </c>
       <c r="K8" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" t="s">
+        <v>0</v>
+      </c>
+      <c r="F9" t="s">
+        <v>0</v>
+      </c>
+      <c r="G9" t="s">
+        <v>0</v>
+      </c>
+      <c r="H9" t="s">
+        <v>16</v>
+      </c>
+      <c r="I9" t="s">
+        <v>0</v>
+      </c>
+      <c r="J9" t="s">
+        <v>0</v>
+      </c>
+      <c r="K9" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" t="s">
+        <v>0</v>
+      </c>
+      <c r="F10" t="s">
+        <v>0</v>
+      </c>
+      <c r="G10" t="s">
+        <v>0</v>
+      </c>
+      <c r="H10" t="s">
+        <v>20</v>
+      </c>
+      <c r="I10" t="s">
+        <v>0</v>
+      </c>
+      <c r="J10" t="s">
+        <v>0</v>
+      </c>
+      <c r="K10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" t="s">
+        <v>0</v>
+      </c>
+      <c r="F11" t="s">
+        <v>0</v>
+      </c>
+      <c r="G11" t="s">
+        <v>0</v>
+      </c>
+      <c r="H11" t="s">
+        <v>24</v>
+      </c>
+      <c r="I11" t="s">
+        <v>0</v>
+      </c>
+      <c r="J11" t="s">
+        <v>0</v>
+      </c>
+      <c r="K11" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" t="s">
+        <v>0</v>
+      </c>
+      <c r="F12" t="s">
+        <v>0</v>
+      </c>
+      <c r="G12" t="s">
+        <v>0</v>
+      </c>
+      <c r="H12" t="s">
+        <v>28</v>
+      </c>
+      <c r="I12" t="s">
+        <v>0</v>
+      </c>
+      <c r="J12" t="s">
+        <v>0</v>
+      </c>
+      <c r="K12" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13" t="s">
+        <v>0</v>
+      </c>
+      <c r="F13" t="s">
+        <v>0</v>
+      </c>
+      <c r="G13" t="s">
+        <v>0</v>
+      </c>
+      <c r="H13" t="s">
+        <v>32</v>
+      </c>
+      <c r="I13" t="s">
+        <v>0</v>
+      </c>
+      <c r="J13" t="s">
+        <v>0</v>
+      </c>
+      <c r="K13" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" t="s">
+        <v>35</v>
+      </c>
+      <c r="E14" t="s">
+        <v>0</v>
+      </c>
+      <c r="F14" t="s">
+        <v>0</v>
+      </c>
+      <c r="G14" t="s">
+        <v>0</v>
+      </c>
+      <c r="H14" t="s">
+        <v>32</v>
+      </c>
+      <c r="I14" t="s">
+        <v>0</v>
+      </c>
+      <c r="J14" t="s">
+        <v>0</v>
+      </c>
+      <c r="K14" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" t="s">
+        <v>39</v>
+      </c>
+      <c r="E15" t="s">
+        <v>0</v>
+      </c>
+      <c r="F15" t="s">
+        <v>0</v>
+      </c>
+      <c r="G15" t="s">
+        <v>0</v>
+      </c>
+      <c r="H15" t="s">
+        <v>40</v>
+      </c>
+      <c r="I15" t="s">
+        <v>0</v>
+      </c>
+      <c r="J15" t="s">
+        <v>0</v>
+      </c>
+      <c r="K15" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
modified readme & excel
</commit_message>
<xml_diff>
--- a/excel.xlsx
+++ b/excel.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="41">
   <si>
     <t/>
   </si>
@@ -471,10 +471,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K15"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:XFD15"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -759,251 +759,6 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" t="s">
-        <v>15</v>
-      </c>
-      <c r="E9" t="s">
-        <v>0</v>
-      </c>
-      <c r="F9" t="s">
-        <v>0</v>
-      </c>
-      <c r="G9" t="s">
-        <v>0</v>
-      </c>
-      <c r="H9" t="s">
-        <v>16</v>
-      </c>
-      <c r="I9" t="s">
-        <v>0</v>
-      </c>
-      <c r="J9" t="s">
-        <v>0</v>
-      </c>
-      <c r="K9" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" t="s">
-        <v>19</v>
-      </c>
-      <c r="E10" t="s">
-        <v>0</v>
-      </c>
-      <c r="F10" t="s">
-        <v>0</v>
-      </c>
-      <c r="G10" t="s">
-        <v>0</v>
-      </c>
-      <c r="H10" t="s">
-        <v>20</v>
-      </c>
-      <c r="I10" t="s">
-        <v>0</v>
-      </c>
-      <c r="J10" t="s">
-        <v>0</v>
-      </c>
-      <c r="K10" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11" t="s">
-        <v>23</v>
-      </c>
-      <c r="E11" t="s">
-        <v>0</v>
-      </c>
-      <c r="F11" t="s">
-        <v>0</v>
-      </c>
-      <c r="G11" t="s">
-        <v>0</v>
-      </c>
-      <c r="H11" t="s">
-        <v>24</v>
-      </c>
-      <c r="I11" t="s">
-        <v>0</v>
-      </c>
-      <c r="J11" t="s">
-        <v>0</v>
-      </c>
-      <c r="K11" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12" t="s">
-        <v>14</v>
-      </c>
-      <c r="D12" t="s">
-        <v>27</v>
-      </c>
-      <c r="E12" t="s">
-        <v>0</v>
-      </c>
-      <c r="F12" t="s">
-        <v>0</v>
-      </c>
-      <c r="G12" t="s">
-        <v>0</v>
-      </c>
-      <c r="H12" t="s">
-        <v>28</v>
-      </c>
-      <c r="I12" t="s">
-        <v>0</v>
-      </c>
-      <c r="J12" t="s">
-        <v>0</v>
-      </c>
-      <c r="K12" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>29</v>
-      </c>
-      <c r="B13" t="s">
-        <v>30</v>
-      </c>
-      <c r="C13" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" t="s">
-        <v>31</v>
-      </c>
-      <c r="E13" t="s">
-        <v>0</v>
-      </c>
-      <c r="F13" t="s">
-        <v>0</v>
-      </c>
-      <c r="G13" t="s">
-        <v>0</v>
-      </c>
-      <c r="H13" t="s">
-        <v>32</v>
-      </c>
-      <c r="I13" t="s">
-        <v>0</v>
-      </c>
-      <c r="J13" t="s">
-        <v>0</v>
-      </c>
-      <c r="K13" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>33</v>
-      </c>
-      <c r="B14" t="s">
-        <v>34</v>
-      </c>
-      <c r="C14" t="s">
-        <v>14</v>
-      </c>
-      <c r="D14" t="s">
-        <v>35</v>
-      </c>
-      <c r="E14" t="s">
-        <v>0</v>
-      </c>
-      <c r="F14" t="s">
-        <v>0</v>
-      </c>
-      <c r="G14" t="s">
-        <v>0</v>
-      </c>
-      <c r="H14" t="s">
-        <v>32</v>
-      </c>
-      <c r="I14" t="s">
-        <v>0</v>
-      </c>
-      <c r="J14" t="s">
-        <v>0</v>
-      </c>
-      <c r="K14" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>36</v>
-      </c>
-      <c r="B15" t="s">
-        <v>37</v>
-      </c>
-      <c r="C15" t="s">
-        <v>38</v>
-      </c>
-      <c r="D15" t="s">
-        <v>39</v>
-      </c>
-      <c r="E15" t="s">
-        <v>0</v>
-      </c>
-      <c r="F15" t="s">
-        <v>0</v>
-      </c>
-      <c r="G15" t="s">
-        <v>0</v>
-      </c>
-      <c r="H15" t="s">
-        <v>40</v>
-      </c>
-      <c r="I15" t="s">
-        <v>0</v>
-      </c>
-      <c r="J15" t="s">
-        <v>0</v>
-      </c>
-      <c r="K15" t="s">
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>